<commit_message>
stadardize template style, #746
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-collection.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-collection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>River</t>
   </si>
@@ -43,9 +43,6 @@
     <t>end time</t>
   </si>
   <si>
-    <t>temp</t>
-  </si>
-  <si>
     <t>start sec</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>fishing seconds</t>
   </si>
   <si>
-    <t>fishing minutes</t>
-  </si>
-  <si>
     <t>Settings</t>
   </si>
   <si>
@@ -134,6 +128,9 @@
   </si>
   <si>
     <t>Bonell</t>
+  </si>
+  <si>
+    <t>Temperature</t>
   </si>
 </sst>
 </file>
@@ -281,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,8 +458,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -577,6 +580,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -622,7 +634,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -636,6 +648,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -981,95 +996,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A3:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" customWidth="1"/>
+    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="L3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="M3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y3" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1082,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,240 +1124,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="K3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>2020</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="5">
+        <v>123</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+      <c r="H4">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>13.6</v>
+      </c>
+      <c r="R4">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="S4">
+        <v>5000</v>
+      </c>
+      <c r="T4">
+        <v>5000</v>
+      </c>
+      <c r="U4" s="7">
+        <f t="shared" ref="U4:U5" si="0">T4/60</f>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="V4">
+        <v>17</v>
+      </c>
+      <c r="X4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y4">
+        <v>543</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>2020</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="5">
+        <v>123</v>
+      </c>
+      <c r="G5">
+        <v>46</v>
+      </c>
+      <c r="H5">
+        <v>47</v>
+      </c>
+      <c r="I5">
+        <v>46.002000000000002</v>
+      </c>
+      <c r="J5">
+        <v>47.000999999999998</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
-        <v>2020</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="5">
-        <v>123</v>
-      </c>
-      <c r="G2">
-        <v>45</v>
-      </c>
-      <c r="H2">
-        <v>46</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="9">
-        <v>0.5625</v>
-      </c>
-      <c r="P2" s="9">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="Q2" s="10">
-        <v>13.6</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
+      <c r="O5" s="9">
+        <v>0.6875</v>
+      </c>
+      <c r="P5" s="8">
+        <v>0.70763888888888893</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>13.5</v>
+      </c>
+      <c r="R5">
         <v>5000</v>
       </c>
-      <c r="T2">
-        <v>5000</v>
-      </c>
-      <c r="U2" s="7">
-        <f t="shared" ref="U2:U3" si="0">T2/60</f>
-        <v>83.333333333333329</v>
-      </c>
-      <c r="V2">
-        <v>17</v>
-      </c>
-      <c r="X2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y2">
-        <v>543</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
-        <v>2020</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="5">
-        <v>123</v>
-      </c>
-      <c r="G3">
-        <v>46</v>
-      </c>
-      <c r="H3">
-        <v>47</v>
-      </c>
-      <c r="I3">
-        <v>46.002000000000002</v>
-      </c>
-      <c r="J3">
-        <v>47.000999999999998</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="9">
-        <v>0.6875</v>
-      </c>
-      <c r="P3" s="8">
-        <v>0.70763888888888893</v>
-      </c>
-      <c r="Q3" s="10">
-        <v>13.5</v>
-      </c>
-      <c r="R3">
-        <v>5000</v>
-      </c>
-      <c r="S3">
+      <c r="S5">
         <v>5422</v>
       </c>
-      <c r="T3">
+      <c r="T5">
         <v>422</v>
       </c>
-      <c r="U3" s="7">
+      <c r="U5" s="7">
         <f t="shared" si="0"/>
         <v>7.0333333333333332</v>
       </c>
-      <c r="W3">
+      <c r="W5">
         <v>16</v>
       </c>
-      <c r="X3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y3">
+      <c r="X5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5">
         <v>543</v>
       </c>
-      <c r="Z3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="Z5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>

</xml_diff>

<commit_message>
clean up electrofishing parser, #749
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-collection.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-collection.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>River</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t>End Tank</t>
   </si>
 </sst>
 </file>
@@ -996,26 +999,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Y3"/>
+  <dimension ref="A3:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1"/>
-    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -1035,60 +1038,63 @@
         <v>31</v>
       </c>
       <c r="G3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="L3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="O3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="Q3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="R3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="S3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="T3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="U3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="13" t="s">
+      <c r="V3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="W3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="W3" s="13" t="s">
+      <c r="X3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="13" t="s">
+      <c r="Y3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Z3" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1100,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,17 +1119,17 @@
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="12" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="6" max="7" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="13" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
@@ -1135,7 +1141,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="2"/>
+      <c r="L1" s="3"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -1144,14 +1150,15 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="4"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -1171,64 +1178,67 @@
         <v>31</v>
       </c>
       <c r="G3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="L3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="O3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="Q3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="R3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="S3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="T3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="U3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="13" t="s">
+      <c r="V3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="W3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="W3" s="13" t="s">
+      <c r="X3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="13" t="s">
+      <c r="Y3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Z3" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>2020</v>
       </c>
@@ -1247,60 +1257,61 @@
       <c r="F4" s="5">
         <v>123</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5"/>
+      <c r="H4">
         <v>45</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>46</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="9">
+      <c r="P4" s="9">
         <v>0.5625</v>
       </c>
-      <c r="P4" s="9">
+      <c r="Q4" s="9">
         <v>0.64583333333333337</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="R4" s="10">
         <v>13.6</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0</v>
-      </c>
-      <c r="S4">
-        <v>5000</v>
       </c>
       <c r="T4">
         <v>5000</v>
       </c>
-      <c r="U4" s="7">
-        <f t="shared" ref="U4:U5" si="0">T4/60</f>
+      <c r="U4">
+        <v>5000</v>
+      </c>
+      <c r="V4" s="7">
+        <f t="shared" ref="V4:V5" si="0">U4/60</f>
         <v>83.333333333333329</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>17</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>16</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>543</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2020</v>
       </c>
@@ -1319,78 +1330,79 @@
       <c r="F5" s="5">
         <v>123</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5"/>
+      <c r="H5">
         <v>46</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>47</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>46.002000000000002</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>47.000999999999998</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>17</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="9">
+      <c r="P5" s="9">
         <v>0.6875</v>
       </c>
-      <c r="P5" s="8">
+      <c r="Q5" s="8">
         <v>0.70763888888888893</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="R5" s="10">
         <v>13.5</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>5000</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>5422</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>422</v>
       </c>
-      <c r="U5" s="7">
+      <c r="V5" s="7">
         <f t="shared" si="0"/>
         <v>7.0333333333333332</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>16</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>16</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>543</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continue improving parsers, update templates and test data
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-collection.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-collection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>River</t>
   </si>
@@ -76,9 +76,6 @@
     <t>AB</t>
   </si>
   <si>
-    <t>CD, EF, GH</t>
-  </si>
-  <si>
     <t>fished in river</t>
   </si>
   <si>
@@ -118,31 +115,33 @@
     <t>Collection</t>
   </si>
   <si>
-    <t>Fall Parr</t>
-  </si>
-  <si>
-    <t>(WS)</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
-    <t>Bonell</t>
-  </si>
-  <si>
     <t>Temperature</t>
   </si>
   <si>
     <t>End Tank</t>
+  </si>
+  <si>
+    <t>Odell</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>CD, EF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -468,7 +467,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -592,6 +591,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -637,23 +645,28 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1019,82 +1032,82 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="L3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="S3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="13" t="s">
+      <c r="T3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="V3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="W3" s="13" t="s">
+      <c r="W3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="X3" s="13" t="s">
+      <c r="X3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Y3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="13" t="s">
+      <c r="Z3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1109,7 +1122,7 @@
   <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,7 +1139,14 @@
     <col min="13" max="14" width="12.85546875" customWidth="1"/>
     <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" customWidth="1"/>
+    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -1159,91 +1179,91 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="L3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="S3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="13" t="s">
+      <c r="T3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="V3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="W3" s="13" t="s">
+      <c r="W3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="X3" s="13" t="s">
+      <c r="X3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Y3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="13" t="s">
+      <c r="Z3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="7">
         <v>2020</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1251,72 +1271,49 @@
       <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="5">
-        <v>123</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4">
-        <v>45</v>
-      </c>
-      <c r="I4">
-        <v>46</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="14"/>
+      <c r="N4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M4" t="s">
+      <c r="R4">
+        <v>110</v>
+      </c>
+      <c r="T4">
+        <v>4</v>
+      </c>
+      <c r="W4">
+        <v>350</v>
+      </c>
+      <c r="X4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y4">
+        <v>500</v>
+      </c>
+      <c r="Z4" t="s">
         <v>18</v>
-      </c>
-      <c r="N4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="9">
-        <v>0.5625</v>
-      </c>
-      <c r="Q4" s="9">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="R4" s="10">
-        <v>13.6</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>5000</v>
-      </c>
-      <c r="U4">
-        <v>5000</v>
-      </c>
-      <c r="V4" s="7">
-        <f t="shared" ref="V4:V5" si="0">U4/60</f>
-        <v>83.333333333333329</v>
-      </c>
-      <c r="W4">
-        <v>17</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z4">
-        <v>543</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="7">
         <v>2020</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1324,86 +1321,67 @@
       <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="5">
-        <v>123</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5">
-        <v>46</v>
-      </c>
-      <c r="I5">
-        <v>47</v>
-      </c>
-      <c r="J5">
-        <v>46.002000000000002</v>
-      </c>
-      <c r="K5">
-        <v>47.000999999999998</v>
-      </c>
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" s="9">
-        <v>0.6875</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>0.70763888888888893</v>
-      </c>
-      <c r="R5" s="10">
-        <v>13.5</v>
+      <c r="E5" s="14"/>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5">
+        <v>21</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="13">
+        <v>45.549656159192402</v>
+      </c>
+      <c r="K5" s="12">
+        <v>-65.013694691467194</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="N5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5">
+        <v>200</v>
       </c>
       <c r="S5">
-        <v>5000</v>
+        <v>16</v>
       </c>
       <c r="T5">
-        <v>5422</v>
-      </c>
-      <c r="U5">
-        <v>422</v>
-      </c>
-      <c r="V5" s="7">
-        <f t="shared" si="0"/>
-        <v>7.0333333333333332</v>
-      </c>
-      <c r="X5">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <v>788</v>
+      </c>
+      <c r="X5" t="s">
         <v>16</v>
       </c>
-      <c r="Y5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z5">
-        <v>543</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>20</v>
+      <c r="Y5">
+        <v>500</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="8"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="8"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="8"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="8"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="8"/>
+      <c r="W11" s="6"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="8"/>
+      <c r="W12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add comments to parser templates, add column header checks to parsers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-collection.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-collection.xlsx
@@ -9,18 +9,268 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="3" r:id="rId1"/>
-    <sheet name="Sample Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+eg. BSR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+eg. Bonell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+eg. FP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Stoyel, Quentin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Stoyel, Quentin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Stoyel, Quentin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional, eg. AB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional, eg. AB, CD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>River</t>
   </si>
@@ -31,12 +281,6 @@
     <t>site code</t>
   </si>
   <si>
-    <t>crew lead</t>
-  </si>
-  <si>
-    <t>crew</t>
-  </si>
-  <si>
     <t>start time</t>
   </si>
   <si>
@@ -67,21 +311,6 @@
     <t># of salmon observed</t>
   </si>
   <si>
-    <t>SMA</t>
-  </si>
-  <si>
-    <t>DC 36%, 60 Hz</t>
-  </si>
-  <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>fished in river</t>
-  </si>
-  <si>
-    <t>saw 16 fish</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -103,15 +332,6 @@
     <t>End Long</t>
   </si>
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Indian Falls</t>
-  </si>
-  <si>
-    <t>Bridge Site</t>
-  </si>
-  <si>
     <t>Collection</t>
   </si>
   <si>
@@ -124,26 +344,20 @@
     <t>End Tank</t>
   </si>
   <si>
-    <t>Odell</t>
-  </si>
-  <si>
-    <t>FP</t>
-  </si>
-  <si>
-    <t>WS</t>
-  </si>
-  <si>
-    <t>CD, EF</t>
+    <t>Crew</t>
+  </si>
+  <si>
+    <t>Crew lead</t>
+  </si>
+  <si>
+    <t>Optional Fields:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +492,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -597,7 +824,9 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -645,26 +874,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1011,11 +1232,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Z3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,360 +1252,120 @@
     <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+    </row>
     <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="9" t="s">
+      <c r="U3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="V3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="9" t="s">
+      <c r="W3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="X3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="Y3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="Z3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Y3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z3" s="9" t="s">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="T2:Z2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="7" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="13" max="14" width="12.85546875" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="X3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z3" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>2020</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4">
-        <v>13</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
-      <c r="N4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4">
-        <v>110</v>
-      </c>
-      <c r="T4">
-        <v>4</v>
-      </c>
-      <c r="W4">
-        <v>350</v>
-      </c>
-      <c r="X4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y4">
-        <v>500</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>2020</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5">
-        <v>21</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="13">
-        <v>45.549656159192402</v>
-      </c>
-      <c r="K5" s="12">
-        <v>-65.013694691467194</v>
-      </c>
-      <c r="L5" s="14"/>
-      <c r="N5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5">
-        <v>200</v>
-      </c>
-      <c r="S5">
-        <v>16</v>
-      </c>
-      <c r="T5">
-        <v>5</v>
-      </c>
-      <c r="W5">
-        <v>788</v>
-      </c>
-      <c r="X5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y5">
-        <v>500</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="W11" s="6"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="W12" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixes to collections parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-collection.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-collection.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyelq\Desktop\Work\dm_apps\dm_apps\bio_diversity\static\data_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E98C1F9-98D7-4302-B411-65BDB15EE3FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="3" r:id="rId1"/>
@@ -19,13 +20,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
     <author>Stoyel, Quentin</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -38,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -77,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -90,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -103,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="1" shapeId="0">
+    <comment ref="G3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -116,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="1" shapeId="0">
+    <comment ref="H3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -129,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="1" shapeId="0">
+    <comment ref="K3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -142,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="1" shapeId="0">
+    <comment ref="L3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="1" shapeId="0">
+    <comment ref="M3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -168,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="1" shapeId="0">
+    <comment ref="T3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -199,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>River</t>
   </si>
@@ -277,12 +278,15 @@
   </si>
   <si>
     <t>Optional Fields:</t>
+  </si>
+  <si>
+    <t># of salmon released</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -984,6 +988,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1019,6 +1040,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1194,11 +1232,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Y4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,24 +1246,25 @@
     <col min="15" max="15" width="12.5703125" customWidth="1"/>
     <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="S2" s="8" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="9"/>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
       <c r="W2" s="9"/>
       <c r="X2" s="9"/>
-      <c r="Y2" s="10"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="10"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1280,29 +1319,32 @@
       <c r="R3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1317,10 +1359,11 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="S2:Y2"/>
+    <mergeCell ref="T2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>